<commit_message>
Major Steel sector update
Have added: coal DRI kilns at Vndjl. New gas DRI kilns. Pelletiser plant.
Saldanha facility with H2 input.
Updated: steel production. demand. intensity values for BFs.

Added all techs and commodities to setsandmaps.
</commit_message>
<xml_diff>
--- a/SubRes_TMPL/SubRES_GreenExports.xlsx
+++ b/SubRes_TMPL/SubRES_GreenExports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SubRes_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC122AB-60C1-438A-9D5A-9264869DC455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B2E4E6-3BD7-4CBB-9807-D3C6E794D91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="-18360" windowWidth="23460" windowHeight="14985" tabRatio="796" firstSheet="2" activeTab="6" xr2:uid="{E4E4DEB2-CFB1-442C-9FC5-D51D154627BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="796" firstSheet="2" activeTab="6" xr2:uid="{E4E4DEB2-CFB1-442C-9FC5-D51D154627BD}"/>
   </bookViews>
   <sheets>
     <sheet name="ANSv2-692-Home" sheetId="9" r:id="rId1"/>
@@ -397,7 +397,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="332">
   <si>
     <t>Comment</t>
   </si>
@@ -1424,6 +1424,12 @@
   </si>
   <si>
     <t>Green Ammonia to Export Market</t>
+  </si>
+  <si>
+    <t>IISHDRI</t>
+  </si>
+  <si>
+    <t>Green DR Iron</t>
   </si>
 </sst>
 </file>
@@ -2857,7 +2863,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2917,7 +2923,7 @@
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3005,7 +3011,7 @@
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3049,7 +3055,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10145,52 +10151,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId5">
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate"/>
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet"/>
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10220,52 +10226,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId11">
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon"/>
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon"/>
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10322,44 +10328,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet">
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -10367,7 +10348,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1"/>
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10397,44 +10403,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter">
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -10442,7 +10423,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2"/>
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11290,7 +11296,7 @@
       </c>
       <c r="D11" s="12" t="str">
         <f>Commodities_BASE!B12</f>
-        <v>IISHBI</v>
+        <v>IISHDRI</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>324</v>
@@ -11753,18 +11759,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -11773,57 +11804,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11853,43 +11859,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -11898,32 +11879,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12171,7 +12177,7 @@
       </c>
       <c r="E12" s="12" t="str">
         <f>Commodities_BASE!B12</f>
-        <v>IISHBI</v>
+        <v>IISHDRI</v>
       </c>
       <c r="F12" s="12" t="str">
         <f t="shared" si="0"/>
@@ -12190,18 +12196,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233473" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="233479" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="233479" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="233478" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>638175</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>190500</xdr:rowOff>
               </to>
@@ -12210,57 +12241,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233473" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="233478" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233474" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="233477" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233474" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="233475" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="233475" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="233477" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12290,43 +12296,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233477" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="233475" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="233477" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="233478" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>190500</xdr:rowOff>
               </to>
@@ -12335,32 +12316,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233478" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="233475" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233479" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="233474" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233479" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="233474" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="233473" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>638175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="233473" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -14925,8 +14931,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102407" r:id="rId8" name="cmdCommName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102407" r:id="rId8" name="cmdCommName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102402" r:id="rId16" name="cmdProcName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102402" r:id="rId16" name="cmdProcName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -14945,182 +15126,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102402" r:id="rId6" name="cmdProcName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102402" r:id="rId6" name="cmdProcName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102407" r:id="rId14" name="cmdCommName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102407" r:id="rId14" name="cmdCommName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2"/>
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -15269,8 +15275,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet">
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -15289,82 +15370,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets"/>
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -15491,8 +15497,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -15511,232 +15742,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -15800,8 +15806,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet">
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -15820,182 +16001,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16070,8 +16076,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -16090,232 +16321,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16402,8 +16408,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>838200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -16422,232 +16653,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>838200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet"/>
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16724,8 +16730,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet">
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -16744,182 +16925,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17005,8 +17011,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears">
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -17025,232 +17256,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -20181,8 +20187,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet">
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -20201,32 +20232,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets"/>
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -20287,18 +20293,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -20307,7 +20313,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets"/>
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -20337,18 +20343,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit">
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -20357,7 +20363,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit"/>
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -20372,7 +20378,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -20499,10 +20505,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
-        <v>183</v>
+        <v>330</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>171</v>
+        <v>331</v>
       </c>
       <c r="D12" s="175" t="s">
         <v>115</v>
@@ -20639,18 +20645,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -20659,7 +20665,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -20689,18 +20695,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -20709,7 +20715,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -20785,18 +20791,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
+                <xdr:col>3</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -20805,7 +20811,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets"/>
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -20835,18 +20841,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
+                <xdr:col>4</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -20855,7 +20861,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit"/>
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>